<commit_message>
Ajustando para calcular a correlação
</commit_message>
<xml_diff>
--- a/correlacao.xlsx
+++ b/correlacao.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\estatistica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jp160\Desktop\IFMS\PDM\6º semestre\Trabalho 2º Bimestre\correlacao_estatistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ED286F-8AAF-455B-B453-BB9C5D81DDA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Correlação</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>BITCOIN</t>
   </si>
@@ -41,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -90,7 +88,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -102,32 +100,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -152,11 +124,11 @@
     <xf numFmtId="44" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -438,11 +410,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C14"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,13 +426,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
@@ -596,19 +568,11 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3">
-        <f>CORREL(B2:B13,C2:C13)</f>
-        <v>0.69986998433091263</v>
-      </c>
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B14:C14"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>

</xml_diff>